<commit_message>
up file ke hoach
</commit_message>
<xml_diff>
--- a/Ke-hoach-thuc-hien-Do-An-1.xlsx
+++ b/Ke-hoach-thuc-hien-Do-An-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Secret\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\itproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF4F58-7949-4BEC-A233-A0D66460CF82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B7F68B-DB56-4454-A169-AE059F9C7A9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>24/11/2021</t>
   </si>
   <si>
-    <t>Thiết kế website bán rau củ cho người tiêu dùng</t>
-  </si>
-  <si>
     <t>Tạ Quang Sang</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>30/11/2021</t>
+  </si>
+  <si>
+    <t>Thiết kế website bán mô hình</t>
   </si>
 </sst>
 </file>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1316,7 +1316,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
@@ -1332,7 +1332,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="52"/>
       <c r="E3" s="52"/>
@@ -1348,7 +1348,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>15</v>
@@ -1366,7 +1366,7 @@
       <c r="A5" s="36"/>
       <c r="B5" s="37"/>
       <c r="C5" s="50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>15</v>
@@ -1403,10 +1403,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>27</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>11</v>
@@ -1469,7 +1469,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="44"/>
       <c r="D9" s="23" t="s">
@@ -1547,7 +1547,7 @@
         <v>44509</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="29"/>
@@ -1584,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="25">
         <v>44265</v>
@@ -1613,7 +1613,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="22" t="s">
@@ -1627,7 +1627,7 @@
         <v>44296</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="20"/>
@@ -1646,10 +1646,10 @@
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>36</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>37</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="20"/>
@@ -1659,7 +1659,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="21" t="s">
@@ -1672,7 +1672,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="25" t="s">
         <v>24</v>
@@ -1701,7 +1701,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="22" t="s">
@@ -1715,7 +1715,7 @@
         <v>23</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I16" s="15"/>
       <c r="J16" s="20"/>

</xml_diff>